<commit_message>
Atualização automática de SANTA_CRUZ_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/SANTA_CRUZ_DO_SUL.xlsx
+++ b/SANTA_CRUZ_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A731D4-F4EA-445D-A8F6-82EDB3814066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB563880-C26B-4109-AD69-C66028819EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1211,7 +1211,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{40D02137-5DA6-4D34-9A00-4A3374D1EE5C}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4372D6C3-6213-41FC-AC4F-FED7E249A681}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1241,10 +1241,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93072282-3F30-44B1-B95F-35441EED28B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135B5938-B70D-4CA8-B9EF-9C2BE228E425}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1282,7 +1282,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F212F157-E030-4763-A75F-BD7985633015}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE62BB14-FD5A-4E98-9208-C47B4A316DA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1345,7 +1345,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45F29D2-5E7D-4343-8B58-C6C0A6E1DF4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEEEB435-8A38-4CD2-A4F5-AC505143522C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1364,7 +1364,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33DA8162-B490-B55C-438B-81E97A6D70FF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3BF1AA-BB73-D5BD-817F-F2BE7C83583A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1413,7 +1413,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB4767D3-EDA4-9157-71A3-78344225214D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E14EC79-6DDE-256B-E3B6-1D9D7A40A89B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1432,7 +1432,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F6436D6-7364-879D-622C-08634B32B9B9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BAB8A19-3FFB-1F37-3342-25C172A407A2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1463,7 +1463,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1256BE07-5F6A-3593-3786-A00660409FA3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E154A9D-2A15-2B14-38DB-0318884F7FEE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1494,7 +1494,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6F183EB-42A2-93EE-A4E7-A9E37467F57E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59FAE81-2706-35FC-61E8-2C568C61E791}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1537,7 +1537,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F31A31F-444A-45BD-931A-29657A63DDE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E0FC986-E1EC-4266-93A3-16F44ED2C854}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1575,7 +1575,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8935291-4D66-496C-9F76-C478E93B694E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80113BD2-A5AF-4F2D-8C64-EF07B67DF689}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,7 +1618,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F593E79D-A0F8-439C-82FB-13AF4AA5364F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{217D6FBC-2130-415A-B96E-7D581A209577}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1931,7 +1931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEC782D-69A2-4D3D-ACEB-2E40C7CDCFCD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8471E97-5CDD-4A00-97F2-EFC135F9CD4B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>